<commit_message>
commit for translate work log
</commit_message>
<xml_diff>
--- a/src/main/resources/Random_translate.xlsx
+++ b/src/main/resources/Random_translate.xlsx
@@ -4157,7 +4157,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4203,14 +4203,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -4526,8 +4535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A157" sqref="A157"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4544,7 +4553,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="12" customFormat="1">
-      <c r="A1" t="s">
+      <c r="A1" s="16" t="s">
         <v>817</v>
       </c>
       <c r="B1" s="10" t="s">
@@ -4570,7 +4579,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A2" t="s">
+      <c r="A2" s="16" t="s">
         <v>818</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -4594,7 +4603,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A3" t="s">
+      <c r="A3" s="16" t="s">
         <v>819</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4618,7 +4627,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A4" t="s">
+      <c r="A4" s="16" t="s">
         <v>820</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -4642,7 +4651,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A5" t="s">
+      <c r="A5" s="16" t="s">
         <v>821</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -4666,7 +4675,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A6" t="s">
+      <c r="A6" s="16" t="s">
         <v>822</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -4690,7 +4699,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1">
-      <c r="A7" t="s">
+      <c r="A7" s="16" t="s">
         <v>823</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -4714,7 +4723,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1">
-      <c r="A8" t="s">
+      <c r="A8" s="16" t="s">
         <v>824</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4738,7 +4747,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" s="13" customFormat="1">
-      <c r="A9" t="s">
+      <c r="A9" s="16" t="s">
         <v>825</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -4762,7 +4771,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A10" t="s">
+      <c r="A10" s="16" t="s">
         <v>826</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -4786,7 +4795,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" s="13" customFormat="1">
-      <c r="A11" t="s">
+      <c r="A11" s="16" t="s">
         <v>827</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -4810,7 +4819,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" s="13" customFormat="1">
-      <c r="A12" t="s">
+      <c r="A12" s="16" t="s">
         <v>828</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -4834,7 +4843,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A13" t="s">
+      <c r="A13" s="16" t="s">
         <v>829</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -4858,7 +4867,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="13" customFormat="1">
-      <c r="A14" t="s">
+      <c r="A14" s="16" t="s">
         <v>830</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -4882,7 +4891,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A15" t="s">
+      <c r="A15" s="16" t="s">
         <v>831</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -4906,7 +4915,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" s="13" customFormat="1">
-      <c r="A16" t="s">
+      <c r="A16" s="16" t="s">
         <v>832</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -4930,7 +4939,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" s="13" customFormat="1">
-      <c r="A17" t="s">
+      <c r="A17" s="16" t="s">
         <v>833</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -4954,7 +4963,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A18" t="s">
+      <c r="A18" s="16" t="s">
         <v>834</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -4978,7 +4987,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A19" t="s">
+      <c r="A19" s="16" t="s">
         <v>835</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -5002,7 +5011,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A20" t="s">
+      <c r="A20" s="16" t="s">
         <v>836</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -5026,7 +5035,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A21" t="s">
+      <c r="A21" s="16" t="s">
         <v>837</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -5050,7 +5059,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" s="13" customFormat="1">
-      <c r="A22" t="s">
+      <c r="A22" s="16" t="s">
         <v>838</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -5074,7 +5083,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" s="13" customFormat="1">
-      <c r="A23" t="s">
+      <c r="A23" s="16" t="s">
         <v>839</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -5098,6 +5107,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A24" s="15"/>
       <c r="B24" s="2" t="s">
         <v>99</v>
       </c>
@@ -5119,7 +5129,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" s="13" customFormat="1">
-      <c r="A25" t="s">
+      <c r="A25" s="16" t="s">
         <v>840</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -5143,7 +5153,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A26" t="s">
+      <c r="A26" s="16" t="s">
         <v>841</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -5167,6 +5177,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>13</v>
       </c>
@@ -5188,6 +5199,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" s="13" customFormat="1" ht="28">
+      <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
         <v>14</v>
       </c>
@@ -5209,6 +5221,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>15</v>
       </c>
@@ -5230,6 +5243,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" s="13" customFormat="1" ht="42">
+      <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>16</v>
       </c>
@@ -5251,6 +5265,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
         <v>17</v>
       </c>
@@ -5272,6 +5287,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>18</v>
       </c>
@@ -5293,6 +5309,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
         <v>19</v>
       </c>
@@ -5314,6 +5331,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" s="13" customFormat="1" ht="42">
+      <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
         <v>20</v>
       </c>
@@ -5335,6 +5353,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" s="13" customFormat="1" ht="42">
+      <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
         <v>21</v>
       </c>
@@ -5356,6 +5375,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
         <v>22</v>
       </c>
@@ -5377,6 +5397,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
         <v>23</v>
       </c>
@@ -5398,6 +5419,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
         <v>24</v>
       </c>
@@ -5419,6 +5441,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
         <v>25</v>
       </c>
@@ -5440,6 +5463,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
         <v>26</v>
       </c>
@@ -5461,6 +5485,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
         <v>102</v>
       </c>
@@ -5482,6 +5507,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" s="13" customFormat="1" ht="56">
+      <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
         <v>647</v>
       </c>
@@ -5503,7 +5529,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" s="13" customFormat="1">
-      <c r="A43" t="s">
+      <c r="A43" s="16" t="s">
         <v>920</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -5527,7 +5553,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" s="13" customFormat="1">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="17" t="s">
         <v>921</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -5551,7 +5577,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" s="13" customFormat="1">
-      <c r="A45" t="s">
+      <c r="A45" s="16" t="s">
         <v>842</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -5575,7 +5601,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A46" t="s">
+      <c r="A46" s="16" t="s">
         <v>843</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -5599,7 +5625,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A47" t="s">
+      <c r="A47" s="16" t="s">
         <v>844</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -5623,6 +5649,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
         <v>31</v>
       </c>
@@ -5644,7 +5671,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A49" t="s">
+      <c r="A49" s="16" t="s">
         <v>845</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -5668,7 +5695,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" s="13" customFormat="1" ht="28">
-      <c r="A50" t="s">
+      <c r="A50" s="16" t="s">
         <v>846</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -5692,7 +5719,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" s="13" customFormat="1" ht="29">
-      <c r="A51" t="s">
+      <c r="A51" s="16" t="s">
         <v>847</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -5716,7 +5743,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" s="13" customFormat="1" ht="42">
-      <c r="A52" t="s">
+      <c r="A52" s="16" t="s">
         <v>848</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -5740,7 +5767,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A53" t="s">
+      <c r="A53" s="16" t="s">
         <v>849</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -5764,7 +5791,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" s="13" customFormat="1">
-      <c r="A54" t="s">
+      <c r="A54" s="16" t="s">
         <v>850</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -5788,7 +5815,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" s="13" customFormat="1">
-      <c r="A55" t="s">
+      <c r="A55" s="16" t="s">
         <v>851</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -5812,7 +5839,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" s="13" customFormat="1">
-      <c r="A56" t="s">
+      <c r="A56" s="16" t="s">
         <v>852</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -5836,7 +5863,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A57" t="s">
+      <c r="A57" s="16" t="s">
         <v>853</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -5860,7 +5887,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" s="13" customFormat="1">
-      <c r="A58" t="s">
+      <c r="A58" s="16" t="s">
         <v>854</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -5884,7 +5911,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" s="13" customFormat="1">
-      <c r="A59" t="s">
+      <c r="A59" s="16" t="s">
         <v>855</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -5908,7 +5935,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" s="13" customFormat="1">
-      <c r="A60" t="s">
+      <c r="A60" s="16" t="s">
         <v>856</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -5932,7 +5959,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" s="13" customFormat="1">
-      <c r="A61" t="s">
+      <c r="A61" s="16" t="s">
         <v>857</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -5956,7 +5983,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" s="13" customFormat="1">
-      <c r="A62" t="s">
+      <c r="A62" s="16" t="s">
         <v>858</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -5980,7 +6007,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" s="13" customFormat="1">
-      <c r="A63" t="s">
+      <c r="A63" s="16" t="s">
         <v>859</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -6004,7 +6031,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" s="13" customFormat="1">
-      <c r="A64" t="s">
+      <c r="A64" s="16" t="s">
         <v>860</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -6028,7 +6055,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" s="13" customFormat="1">
-      <c r="A65" t="s">
+      <c r="A65" s="16" t="s">
         <v>861</v>
       </c>
       <c r="B65" s="2" t="s">
@@ -6052,7 +6079,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" s="13" customFormat="1">
-      <c r="A66" t="s">
+      <c r="A66" s="16" t="s">
         <v>862</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -6076,7 +6103,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" s="13" customFormat="1">
-      <c r="A67" t="s">
+      <c r="A67" s="16" t="s">
         <v>863</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -6100,7 +6127,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" s="13" customFormat="1">
-      <c r="A68" t="s">
+      <c r="A68" s="16" t="s">
         <v>864</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -6124,7 +6151,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" s="13" customFormat="1">
-      <c r="A69" t="s">
+      <c r="A69" s="16" t="s">
         <v>865</v>
       </c>
       <c r="B69" s="2" t="s">
@@ -6148,7 +6175,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" s="13" customFormat="1">
-      <c r="A70" t="s">
+      <c r="A70" s="16" t="s">
         <v>866</v>
       </c>
       <c r="B70" s="2" t="s">
@@ -6172,7 +6199,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" s="13" customFormat="1">
-      <c r="A71" t="s">
+      <c r="A71" s="16" t="s">
         <v>867</v>
       </c>
       <c r="B71" s="2" t="s">
@@ -6196,7 +6223,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" s="13" customFormat="1">
-      <c r="A72" t="s">
+      <c r="A72" s="16" t="s">
         <v>868</v>
       </c>
       <c r="B72" s="2" t="s">
@@ -6220,7 +6247,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" s="13" customFormat="1">
-      <c r="A73" t="s">
+      <c r="A73" s="16" t="s">
         <v>869</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -6244,7 +6271,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" s="13" customFormat="1">
-      <c r="A74" t="s">
+      <c r="A74" s="16" t="s">
         <v>870</v>
       </c>
       <c r="B74" s="2" t="s">
@@ -6268,7 +6295,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A75" t="s">
+      <c r="A75" s="16" t="s">
         <v>871</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -6292,7 +6319,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A76" t="s">
+      <c r="A76" s="16" t="s">
         <v>872</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -6316,7 +6343,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" s="13" customFormat="1">
-      <c r="A77" t="s">
+      <c r="A77" s="16" t="s">
         <v>873</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -6340,7 +6367,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A78" t="s">
+      <c r="A78" s="16" t="s">
         <v>874</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -6364,7 +6391,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A79" t="s">
+      <c r="A79" s="16" t="s">
         <v>875</v>
       </c>
       <c r="B79" s="2" t="s">
@@ -6388,7 +6415,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A80" t="s">
+      <c r="A80" s="16" t="s">
         <v>876</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -6412,7 +6439,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A81" t="s">
+      <c r="A81" s="16" t="s">
         <v>877</v>
       </c>
       <c r="B81" s="2" t="s">
@@ -6436,7 +6463,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" s="13" customFormat="1" ht="29">
-      <c r="A82" t="s">
+      <c r="A82" s="16" t="s">
         <v>878</v>
       </c>
       <c r="B82" s="2" t="s">
@@ -6460,7 +6487,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" s="13" customFormat="1" ht="84">
-      <c r="A83" t="s">
+      <c r="A83" s="16" t="s">
         <v>879</v>
       </c>
       <c r="B83" s="2" t="s">
@@ -6484,7 +6511,7 @@
       </c>
     </row>
     <row r="84" spans="1:8" s="13" customFormat="1">
-      <c r="A84" t="s">
+      <c r="A84" s="16" t="s">
         <v>880</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -6508,7 +6535,7 @@
       </c>
     </row>
     <row r="85" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A85" t="s">
+      <c r="A85" s="16" t="s">
         <v>881</v>
       </c>
       <c r="B85" s="2" t="s">
@@ -6532,7 +6559,7 @@
       </c>
     </row>
     <row r="86" spans="1:8" s="13" customFormat="1" ht="28">
-      <c r="A86" t="s">
+      <c r="A86" s="16" t="s">
         <v>882</v>
       </c>
       <c r="B86" s="2" t="s">
@@ -6556,7 +6583,7 @@
       </c>
     </row>
     <row r="87" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A87" t="s">
+      <c r="A87" s="16" t="s">
         <v>883</v>
       </c>
       <c r="B87" s="2" t="s">
@@ -6580,7 +6607,7 @@
       </c>
     </row>
     <row r="88" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A88" t="s">
+      <c r="A88" s="16" t="s">
         <v>884</v>
       </c>
       <c r="B88" s="2" t="s">
@@ -6604,7 +6631,7 @@
       </c>
     </row>
     <row r="89" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A89" t="s">
+      <c r="A89" s="16" t="s">
         <v>885</v>
       </c>
       <c r="B89" s="2" t="s">
@@ -6628,7 +6655,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A90" t="s">
+      <c r="A90" s="16" t="s">
         <v>886</v>
       </c>
       <c r="B90" s="2" t="s">
@@ -6652,7 +6679,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" s="13" customFormat="1" ht="28">
-      <c r="A91" t="s">
+      <c r="A91" s="16" t="s">
         <v>887</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -6676,7 +6703,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" s="13" customFormat="1" ht="56">
-      <c r="A92" t="s">
+      <c r="A92" s="16" t="s">
         <v>888</v>
       </c>
       <c r="B92" s="2" t="s">
@@ -6700,7 +6727,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" s="13" customFormat="1" ht="29">
-      <c r="A93" t="s">
+      <c r="A93" s="16" t="s">
         <v>889</v>
       </c>
       <c r="B93" s="2" t="s">
@@ -6724,7 +6751,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" s="13" customFormat="1" ht="29">
-      <c r="A94" t="s">
+      <c r="A94" s="16" t="s">
         <v>890</v>
       </c>
       <c r="B94" s="2" t="s">
@@ -6748,7 +6775,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" s="13" customFormat="1" ht="29">
-      <c r="A95" t="s">
+      <c r="A95" s="16" t="s">
         <v>891</v>
       </c>
       <c r="B95" s="2" t="s">
@@ -6772,7 +6799,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A96" t="s">
+      <c r="A96" s="16" t="s">
         <v>892</v>
       </c>
       <c r="B96" s="2" t="s">
@@ -6796,7 +6823,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" s="13" customFormat="1" ht="70">
-      <c r="A97" t="s">
+      <c r="A97" s="16" t="s">
         <v>893</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -6820,7 +6847,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A98" t="s">
+      <c r="A98" s="16" t="s">
         <v>894</v>
       </c>
       <c r="B98" s="2" t="s">
@@ -6844,6 +6871,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A99" s="2"/>
       <c r="B99" s="2" t="s">
         <v>650</v>
       </c>
@@ -6865,6 +6893,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A100" s="2"/>
       <c r="B100" s="2" t="s">
         <v>60</v>
       </c>
@@ -6886,6 +6915,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A101" s="2"/>
       <c r="B101" s="2" t="s">
         <v>61</v>
       </c>
@@ -6907,6 +6937,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" s="13" customFormat="1" ht="42">
+      <c r="A102" s="2"/>
       <c r="B102" s="2" t="s">
         <v>310</v>
       </c>
@@ -6928,6 +6959,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" s="13" customFormat="1" ht="42">
+      <c r="A103" s="2"/>
       <c r="B103" s="2" t="s">
         <v>316</v>
       </c>
@@ -6949,6 +6981,7 @@
       </c>
     </row>
     <row r="104" spans="1:8" s="13" customFormat="1" ht="42">
+      <c r="A104" s="2"/>
       <c r="B104" s="2" t="s">
         <v>317</v>
       </c>
@@ -6970,6 +7003,7 @@
       </c>
     </row>
     <row r="105" spans="1:8" s="13" customFormat="1" ht="56">
+      <c r="A105" s="2"/>
       <c r="B105" s="2" t="s">
         <v>311</v>
       </c>
@@ -6991,6 +7025,7 @@
       </c>
     </row>
     <row r="106" spans="1:8" s="13" customFormat="1" ht="56">
+      <c r="A106" s="2"/>
       <c r="B106" s="2" t="s">
         <v>309</v>
       </c>
@@ -7012,6 +7047,7 @@
       </c>
     </row>
     <row r="107" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A107" s="2"/>
       <c r="B107" s="2" t="s">
         <v>62</v>
       </c>
@@ -7033,6 +7069,7 @@
       </c>
     </row>
     <row r="108" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A108" s="2"/>
       <c r="B108" s="2" t="s">
         <v>63</v>
       </c>
@@ -7054,6 +7091,7 @@
       </c>
     </row>
     <row r="109" spans="1:8" s="13" customFormat="1" ht="84">
+      <c r="A109" s="2"/>
       <c r="B109" s="2" t="s">
         <v>64</v>
       </c>
@@ -7075,6 +7113,7 @@
       </c>
     </row>
     <row r="110" spans="1:8" s="13" customFormat="1" ht="28">
+      <c r="A110" s="2"/>
       <c r="B110" s="2" t="s">
         <v>65</v>
       </c>
@@ -7096,6 +7135,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" s="13" customFormat="1" ht="28">
+      <c r="A111" s="2"/>
       <c r="B111" s="2" t="s">
         <v>66</v>
       </c>
@@ -7117,6 +7157,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" s="13" customFormat="1" ht="28">
+      <c r="A112" s="2"/>
       <c r="B112" s="2" t="s">
         <v>67</v>
       </c>
@@ -7138,6 +7179,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A113" s="2"/>
       <c r="B113" s="2" t="s">
         <v>303</v>
       </c>
@@ -7159,6 +7201,7 @@
       </c>
     </row>
     <row r="114" spans="1:8" s="13" customFormat="1" ht="28">
+      <c r="A114" s="2"/>
       <c r="B114" s="2" t="s">
         <v>305</v>
       </c>
@@ -7180,6 +7223,7 @@
       </c>
     </row>
     <row r="115" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A115" s="2"/>
       <c r="B115" s="2" t="s">
         <v>128</v>
       </c>
@@ -7201,6 +7245,7 @@
       </c>
     </row>
     <row r="116" spans="1:8" s="13" customFormat="1" ht="28">
+      <c r="A116" s="2"/>
       <c r="B116" s="2" t="s">
         <v>68</v>
       </c>
@@ -7222,7 +7267,7 @@
       </c>
     </row>
     <row r="117" spans="1:8" s="13" customFormat="1" ht="29">
-      <c r="A117" t="s">
+      <c r="A117" s="16" t="s">
         <v>895</v>
       </c>
       <c r="B117" s="2" t="s">
@@ -7246,7 +7291,7 @@
       </c>
     </row>
     <row r="118" spans="1:8" s="13" customFormat="1" ht="42">
-      <c r="A118" t="s">
+      <c r="A118" s="16" t="s">
         <v>896</v>
       </c>
       <c r="B118" s="2" t="s">
@@ -7270,7 +7315,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A119" t="s">
+      <c r="A119" s="16" t="s">
         <v>897</v>
       </c>
       <c r="B119" s="2" t="s">
@@ -7294,7 +7339,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" s="13" customFormat="1" ht="42">
-      <c r="A120" t="s">
+      <c r="A120" s="16" t="s">
         <v>898</v>
       </c>
       <c r="B120" s="2" t="s">
@@ -7318,7 +7363,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" s="13" customFormat="1" ht="29">
-      <c r="A121" t="s">
+      <c r="A121" s="16" t="s">
         <v>899</v>
       </c>
       <c r="B121" s="2" t="s">
@@ -7342,7 +7387,7 @@
       </c>
     </row>
     <row r="122" spans="1:8" s="13" customFormat="1" ht="42">
-      <c r="A122" t="s">
+      <c r="A122" s="16" t="s">
         <v>900</v>
       </c>
       <c r="B122" s="2" t="s">
@@ -7366,7 +7411,7 @@
       </c>
     </row>
     <row r="123" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A123" t="s">
+      <c r="A123" s="16" t="s">
         <v>901</v>
       </c>
       <c r="B123" s="2" t="s">
@@ -7390,7 +7435,7 @@
       </c>
     </row>
     <row r="124" spans="1:8" s="13" customFormat="1" ht="42">
-      <c r="A124" t="s">
+      <c r="A124" s="16" t="s">
         <v>902</v>
       </c>
       <c r="B124" s="2" t="s">
@@ -7414,6 +7459,7 @@
       </c>
     </row>
     <row r="125" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A125" s="2"/>
       <c r="B125" s="2" t="s">
         <v>129</v>
       </c>
@@ -7435,6 +7481,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" s="13" customFormat="1" ht="42">
+      <c r="A126" s="2"/>
       <c r="B126" s="2" t="s">
         <v>130</v>
       </c>
@@ -7456,6 +7503,7 @@
       </c>
     </row>
     <row r="127" spans="1:8" s="13" customFormat="1" ht="28">
+      <c r="A127" s="2"/>
       <c r="B127" s="2" t="s">
         <v>131</v>
       </c>
@@ -7477,6 +7525,7 @@
       </c>
     </row>
     <row r="128" spans="1:8" s="13" customFormat="1" ht="42">
+      <c r="A128" s="2"/>
       <c r="B128" s="2" t="s">
         <v>132</v>
       </c>
@@ -7498,7 +7547,7 @@
       </c>
     </row>
     <row r="129" spans="1:8" s="13" customFormat="1" ht="28">
-      <c r="A129" t="s">
+      <c r="A129" s="16" t="s">
         <v>903</v>
       </c>
       <c r="B129" s="2" t="s">
@@ -7522,7 +7571,7 @@
       </c>
     </row>
     <row r="130" spans="1:8" s="13" customFormat="1" ht="56">
-      <c r="A130" t="s">
+      <c r="A130" s="16" t="s">
         <v>904</v>
       </c>
       <c r="B130" s="2" t="s">
@@ -7546,6 +7595,7 @@
       </c>
     </row>
     <row r="131" spans="1:8" s="13" customFormat="1" ht="42">
+      <c r="A131" s="2"/>
       <c r="B131" s="2" t="s">
         <v>78</v>
       </c>
@@ -7567,6 +7617,7 @@
       </c>
     </row>
     <row r="132" spans="1:8" s="13" customFormat="1" ht="17">
+      <c r="A132" s="2"/>
       <c r="B132" s="2" t="s">
         <v>79</v>
       </c>
@@ -7588,7 +7639,7 @@
       </c>
     </row>
     <row r="133" spans="1:8" s="13" customFormat="1" ht="42">
-      <c r="A133" t="s">
+      <c r="A133" s="16" t="s">
         <v>905</v>
       </c>
       <c r="B133" s="2" t="s">
@@ -7612,6 +7663,7 @@
       </c>
     </row>
     <row r="134" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A134" s="2"/>
       <c r="B134" s="2" t="s">
         <v>80</v>
       </c>
@@ -7633,6 +7685,7 @@
       </c>
     </row>
     <row r="135" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A135" s="2"/>
       <c r="B135" s="2" t="s">
         <v>81</v>
       </c>
@@ -7654,6 +7707,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" s="13" customFormat="1" ht="84">
+      <c r="A136" s="2"/>
       <c r="B136" s="2" t="s">
         <v>649</v>
       </c>
@@ -7675,7 +7729,7 @@
       </c>
     </row>
     <row r="137" spans="1:8" s="13" customFormat="1">
-      <c r="A137" t="s">
+      <c r="A137" s="16" t="s">
         <v>906</v>
       </c>
       <c r="B137" s="3" t="s">
@@ -7699,7 +7753,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" s="13" customFormat="1">
-      <c r="A138" t="s">
+      <c r="A138" s="16" t="s">
         <v>907</v>
       </c>
       <c r="B138" s="3" t="s">
@@ -7723,6 +7777,7 @@
       </c>
     </row>
     <row r="139" spans="1:8" s="13" customFormat="1" ht="42">
+      <c r="A139" s="2"/>
       <c r="B139" s="3" t="s">
         <v>137</v>
       </c>
@@ -7744,6 +7799,7 @@
       </c>
     </row>
     <row r="140" spans="1:8" s="13" customFormat="1" ht="29">
+      <c r="A140" s="2"/>
       <c r="B140" s="3" t="s">
         <v>138</v>
       </c>
@@ -7765,7 +7821,7 @@
       </c>
     </row>
     <row r="141" spans="1:8" s="13" customFormat="1" ht="28">
-      <c r="A141" t="s">
+      <c r="A141" s="16" t="s">
         <v>908</v>
       </c>
       <c r="B141" s="3" t="s">
@@ -7789,6 +7845,7 @@
       </c>
     </row>
     <row r="142" spans="1:8" s="13" customFormat="1">
+      <c r="A142" s="2"/>
       <c r="B142" s="3" t="s">
         <v>139</v>
       </c>
@@ -7810,6 +7867,7 @@
       </c>
     </row>
     <row r="143" spans="1:8" s="13" customFormat="1">
+      <c r="A143" s="2"/>
       <c r="B143" s="3" t="s">
         <v>140</v>
       </c>
@@ -7831,7 +7889,7 @@
       </c>
     </row>
     <row r="144" spans="1:8" s="13" customFormat="1" ht="17">
-      <c r="A144" t="s">
+      <c r="A144" s="16" t="s">
         <v>909</v>
       </c>
       <c r="B144" s="3" t="s">
@@ -7855,7 +7913,7 @@
       </c>
     </row>
     <row r="145" spans="1:12" s="13" customFormat="1" ht="28">
-      <c r="A145" t="s">
+      <c r="A145" s="16" t="s">
         <v>910</v>
       </c>
       <c r="B145" s="3" t="s">
@@ -7879,7 +7937,7 @@
       </c>
     </row>
     <row r="146" spans="1:12" s="13" customFormat="1" ht="56">
-      <c r="A146" t="s">
+      <c r="A146" s="16" t="s">
         <v>911</v>
       </c>
       <c r="B146" s="3" t="s">
@@ -7903,7 +7961,7 @@
       </c>
     </row>
     <row r="147" spans="1:12" s="13" customFormat="1">
-      <c r="A147" t="s">
+      <c r="A147" s="16" t="s">
         <v>912</v>
       </c>
       <c r="B147" s="3" t="s">
@@ -7927,7 +7985,7 @@
       </c>
     </row>
     <row r="148" spans="1:12" s="13" customFormat="1" ht="28">
-      <c r="A148" t="s">
+      <c r="A148" s="16" t="s">
         <v>913</v>
       </c>
       <c r="B148" s="3" t="s">
@@ -7951,6 +8009,7 @@
       </c>
     </row>
     <row r="149" spans="1:12" s="13" customFormat="1" ht="28">
+      <c r="A149" s="2"/>
       <c r="B149" s="3" t="s">
         <v>146</v>
       </c>
@@ -7972,7 +8031,7 @@
       </c>
     </row>
     <row r="150" spans="1:12" s="13" customFormat="1">
-      <c r="A150" t="s">
+      <c r="A150" s="16" t="s">
         <v>914</v>
       </c>
       <c r="B150" s="3" t="s">
@@ -7996,7 +8055,7 @@
       </c>
     </row>
     <row r="151" spans="1:12" s="13" customFormat="1">
-      <c r="A151" t="s">
+      <c r="A151" s="16" t="s">
         <v>915</v>
       </c>
       <c r="B151" s="3" t="s">
@@ -8020,7 +8079,7 @@
       </c>
     </row>
     <row r="152" spans="1:12" s="13" customFormat="1">
-      <c r="A152" t="s">
+      <c r="A152" s="16" t="s">
         <v>916</v>
       </c>
       <c r="B152" s="3" t="s">
@@ -8044,7 +8103,7 @@
       </c>
     </row>
     <row r="153" spans="1:12" s="13" customFormat="1" ht="28">
-      <c r="A153" t="s">
+      <c r="A153" s="16" t="s">
         <v>917</v>
       </c>
       <c r="B153" s="3" t="s">
@@ -8068,7 +8127,7 @@
       </c>
     </row>
     <row r="154" spans="1:12" s="13" customFormat="1" ht="29">
-      <c r="A154" t="s">
+      <c r="A154" s="16" t="s">
         <v>918</v>
       </c>
       <c r="B154" s="3" t="s">
@@ -8092,7 +8151,7 @@
       </c>
     </row>
     <row r="155" spans="1:12" s="13" customFormat="1" ht="17">
-      <c r="A155" t="s">
+      <c r="A155" s="16" t="s">
         <v>922</v>
       </c>
       <c r="B155" s="3" t="s">
@@ -8116,7 +8175,7 @@
       </c>
     </row>
     <row r="156" spans="1:12" s="13" customFormat="1" ht="17">
-      <c r="A156" t="s">
+      <c r="A156" s="16" t="s">
         <v>919</v>
       </c>
       <c r="B156" s="3" t="s">
@@ -8140,7 +8199,7 @@
       </c>
     </row>
     <row r="157" spans="1:12" s="13" customFormat="1" ht="196">
-      <c r="A157" t="s">
+      <c r="A157" s="16" t="s">
         <v>927</v>
       </c>
       <c r="B157" s="3" t="s">
@@ -8164,7 +8223,7 @@
       </c>
     </row>
     <row r="158" spans="1:12" s="13" customFormat="1" ht="168">
-      <c r="A158" t="s">
+      <c r="A158" s="16" t="s">
         <v>926</v>
       </c>
       <c r="B158" s="3" t="s">
@@ -8188,6 +8247,7 @@
       </c>
     </row>
     <row r="159" spans="1:12" s="13" customFormat="1" ht="17">
+      <c r="A159" s="2"/>
       <c r="B159" s="3" t="s">
         <v>155</v>
       </c>
@@ -8209,7 +8269,7 @@
       </c>
     </row>
     <row r="160" spans="1:12" s="13" customFormat="1" ht="126">
-      <c r="A160" s="17" t="s">
+      <c r="A160" s="18" t="s">
         <v>925</v>
       </c>
       <c r="B160" s="3" t="s">
@@ -8237,7 +8297,7 @@
       <c r="L160" s="1"/>
     </row>
     <row r="161" spans="1:8">
-      <c r="A161" s="16" t="s">
+      <c r="A161" s="19" t="s">
         <v>923</v>
       </c>
       <c r="B161" s="3" t="s">
@@ -8261,7 +8321,7 @@
       </c>
     </row>
     <row r="162" spans="1:8">
-      <c r="A162" s="16" t="s">
+      <c r="A162" s="19" t="s">
         <v>924</v>
       </c>
       <c r="B162" s="3" t="s">
@@ -8285,6 +8345,7 @@
       </c>
     </row>
     <row r="163" spans="1:8" ht="42">
+      <c r="A163" s="20"/>
       <c r="B163" s="3" t="s">
         <v>651</v>
       </c>

</xml_diff>